<commit_message>
MàJ armes françaises (F17P et F21)
</commit_message>
<xml_diff>
--- a/Docs/Armements Cold Waters.xlsx
+++ b/Docs/Armements Cold Waters.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{62ED53D6-2E18-4BCC-8872-D5E530CD4588}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12,14 +13,14 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$F$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$F$40</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
   <si>
     <t>Armements</t>
   </si>
@@ -205,12 +206,21 @@
   </si>
   <si>
     <t>50 - 65</t>
+  </si>
+  <si>
+    <t>F17P</t>
+  </si>
+  <si>
+    <t>F21</t>
+  </si>
+  <si>
+    <t>50 - 60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -375,6 +385,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -422,7 +435,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -455,9 +468,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -490,6 +520,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -665,13 +712,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -715,7 +764,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" s="18" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="18" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>1</v>
       </c>
@@ -735,7 +784,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>48</v>
       </c>
@@ -755,7 +804,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>58</v>
       </c>
@@ -775,7 +824,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
@@ -795,7 +844,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>60</v>
       </c>
@@ -815,105 +864,127 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>7</v>
+        <v>62</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="C10" s="9">
-        <v>15</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="9">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="D10" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6">
+        <v>65</v>
+      </c>
+      <c r="D11" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="9">
+        <v>15</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="9">
+        <v>20</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="D11" s="16">
-        <v>30</v>
-      </c>
-      <c r="E11" s="6">
-        <v>466</v>
-      </c>
-      <c r="F11" s="6">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="15">
-        <v>30</v>
-      </c>
-      <c r="E12" s="9">
-        <v>490</v>
-      </c>
-      <c r="F12" s="9">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="D13" s="16">
         <v>30</v>
       </c>
       <c r="E13" s="6">
-        <v>490</v>
+        <v>466</v>
       </c>
       <c r="F13" s="6">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="15">
+        <v>30</v>
+      </c>
+      <c r="E14" s="9">
+        <v>490</v>
+      </c>
+      <c r="F14" s="9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="16">
+        <v>30</v>
+      </c>
+      <c r="E15" s="6">
+        <v>490</v>
+      </c>
+      <c r="F15" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="7"/>
@@ -921,377 +992,357 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="13">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="D17" s="22">
-        <v>0.88</v>
-      </c>
-      <c r="E17" s="9">
-        <v>29</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="14">
-        <v>17.5</v>
-      </c>
-      <c r="D18" s="23">
-        <v>0.88</v>
-      </c>
-      <c r="E18" s="12">
-        <v>40</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="13">
-        <v>17.5</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D19" s="22">
-        <v>1.5</v>
+        <v>0.88</v>
       </c>
       <c r="E19" s="9">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="14">
-        <v>22</v>
+        <v>17.5</v>
       </c>
       <c r="D20" s="23">
-        <v>3</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>30</v>
+        <v>0.88</v>
+      </c>
+      <c r="E20" s="12">
+        <v>40</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="13">
-        <v>27.3</v>
+        <v>17.5</v>
       </c>
       <c r="D21" s="22">
-        <v>0.88</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>26</v>
+        <v>1.5</v>
+      </c>
+      <c r="E21" s="9">
+        <v>40</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="14">
-        <v>27.3</v>
+        <v>22</v>
       </c>
       <c r="D22" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="13">
+        <v>27.3</v>
+      </c>
+      <c r="D23" s="22">
+        <v>0.88</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="14">
+        <v>27.3</v>
+      </c>
+      <c r="D24" s="23">
+        <v>2</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="13">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="D23" s="22">
-        <v>1.65</v>
-      </c>
-      <c r="E23" s="9">
-        <v>41</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="14">
-        <v>5.5</v>
-      </c>
-      <c r="D24" s="23">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E24" s="12">
-        <v>27</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="13">
-        <v>7.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D25" s="22">
-        <v>1.1000000000000001</v>
+        <v>1.65</v>
       </c>
       <c r="E25" s="9">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="14">
+        <v>5.5</v>
+      </c>
+      <c r="D26" s="23">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E26" s="12">
+        <v>27</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="13">
+        <v>7.7</v>
+      </c>
+      <c r="D27" s="22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E27" s="9">
+        <v>40</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B28" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C28" s="14">
         <v>55</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D28" s="23">
         <v>4</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E28" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="13">
-        <v>55</v>
-      </c>
-      <c r="D27" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="23">
-        <v>0.12</v>
-      </c>
-      <c r="E28" s="25" t="s">
-        <v>25</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="29" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="13">
+        <v>55</v>
+      </c>
+      <c r="D29" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+    <row r="33" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="13">
-        <v>9</v>
-      </c>
-      <c r="D32" s="22">
-        <v>0.8</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="14">
-        <v>18</v>
-      </c>
-      <c r="D33" s="23">
-        <v>1.6</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="13">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D34" s="22">
-        <v>1.6</v>
-      </c>
-      <c r="E34" s="9">
-        <v>43</v>
+        <v>0.8</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C35" s="14">
         <v>18</v>
       </c>
       <c r="D35" s="23">
+        <v>1.6</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="13">
+        <v>8</v>
+      </c>
+      <c r="D36" s="22">
+        <v>1.6</v>
+      </c>
+      <c r="E36" s="9">
+        <v>43</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="14">
+        <v>18</v>
+      </c>
+      <c r="D37" s="23">
         <v>1.5</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E37" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F37" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+    <row r="38" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B38" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="22">
-        <v>0.12</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="23">
-        <v>0.1</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>25</v>
@@ -1306,14 +1357,54 @@
         <v>36</v>
       </c>
     </row>
+    <row r="39" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="22">
+        <v>0.12</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.59055118110236227" right="3.937007874015748E-2" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="94" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="93" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1325,7 +1416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>